<commit_message>
Equal score rules added
</commit_message>
<xml_diff>
--- a/docs/OrdinePartenzaFinale.xlsx
+++ b/docs/OrdinePartenzaFinale.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\MemorialGander\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
     <sheet name="F" sheetId="2" r:id="rId2"/>
     <sheet name="M+F" sheetId="3" r:id="rId3"/>
+    <sheet name="Apparatus" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">F!$A$4:$C$13</definedName>
@@ -31,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>Arthur Nory Mariano</t>
-  </si>
-  <si>
     <t xml:space="preserve">Benjamin Gischard  </t>
   </si>
   <si>
@@ -48,33 +46,18 @@
     <t xml:space="preserve">Igor Radivilov     </t>
   </si>
   <si>
-    <t xml:space="preserve">Lucas Dauser       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Marian Dragulescu  </t>
   </si>
   <si>
     <t xml:space="preserve">Marco Rizzo        </t>
   </si>
   <si>
-    <t xml:space="preserve">Nikita Ignatyev    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Oleg Verniaiev     </t>
   </si>
   <si>
-    <t xml:space="preserve">Paolo Principi     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">René Cournoyer     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Angelina Melnikova </t>
   </si>
   <si>
-    <t xml:space="preserve">Angelina Kysla     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Caterina Barloggio </t>
   </si>
   <si>
@@ -90,12 +73,6 @@
     <t xml:space="preserve">J.B Lopez Arocha   </t>
   </si>
   <si>
-    <t xml:space="preserve">Thea Brogli        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victoria Kayen Woo </t>
-  </si>
-  <si>
     <t>Parallel bars</t>
   </si>
   <si>
@@ -130,6 +107,87 @@
   </si>
   <si>
     <t>Balance Beam</t>
+  </si>
+  <si>
+    <t>Arthur Nory Oyakawa Mariano</t>
+  </si>
+  <si>
+    <t>Bart Deurloo</t>
+  </si>
+  <si>
+    <t>James Hall</t>
+  </si>
+  <si>
+    <t>Marcel Nguyen</t>
+  </si>
+  <si>
+    <t>Marian Dragulescu</t>
+  </si>
+  <si>
+    <t>Nikita Nagornyy</t>
+  </si>
+  <si>
+    <t>Oleg Verniaiev</t>
+  </si>
+  <si>
+    <t>Oliver Hegi</t>
+  </si>
+  <si>
+    <t>Cory Paterson</t>
+  </si>
+  <si>
+    <t>Pablo Brägger</t>
+  </si>
+  <si>
+    <t>Julien Gobaux</t>
+  </si>
+  <si>
+    <t>Thea Brogli</t>
+  </si>
+  <si>
+    <t>Angelina Melnikova</t>
+  </si>
+  <si>
+    <t>Diana Varinska</t>
+  </si>
+  <si>
+    <t>Emily Thomas</t>
+  </si>
+  <si>
+    <t>Ilaria Kaeslin</t>
+  </si>
+  <si>
+    <t>Isabela Onyshko</t>
+  </si>
+  <si>
+    <t>Kim Bui Germany</t>
+  </si>
+  <si>
+    <t>Leonie Meier</t>
+  </si>
+  <si>
+    <t>Mélanie De Jesus Dos Santos</t>
+  </si>
+  <si>
+    <t>Oksana Chusovitina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flávia Lopes Saraiva </t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Parallel Bars</t>
+  </si>
+  <si>
+    <t>Horizontal Bar</t>
+  </si>
+  <si>
+    <t>Pommel Horse</t>
   </si>
 </sst>
 </file>
@@ -191,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -207,6 +265,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,21 +582,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="25.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.75" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,10 +604,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -556,9 +615,6 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -567,10 +623,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -578,10 +631,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -589,10 +639,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,10 +647,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,50 +655,32 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -665,6 +691,18 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Apparatus!$A$4:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -673,7 +711,7 @@
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -686,7 +724,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,10 +732,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,10 +743,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,10 +751,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,10 +759,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,10 +767,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,10 +775,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,47 +783,44 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -813,6 +833,18 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Apparatus!$A$12:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -820,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -833,7 +865,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -848,10 +880,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -859,10 +891,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -870,10 +902,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -881,10 +913,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -892,10 +924,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -903,10 +935,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -914,10 +946,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -947,7 +979,7 @@
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -962,10 +994,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -973,10 +1005,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -984,10 +1016,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -995,10 +1027,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1006,10 +1038,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1017,10 +1049,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1028,10 +1060,10 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1053,4 +1085,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data for edition 2018 added
- Lollo's improvements so that is nolonger necessary to copy from tab to tab
</commit_message>
<xml_diff>
--- a/docs/OrdinePartenzaFinale.xlsx
+++ b/docs/OrdinePartenzaFinale.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\MemorialGander\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0amalor\Work folders\Roaming\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6934A617-D059-4EBB-9233-AF2F18726A3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">M!$A$4:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'M+F'!$A$4:$C$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,62 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t xml:space="preserve">Benjamin Gischard  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bart Deurloo       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Igor Radivilov     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marian Dragulescu  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marco Rizzo        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oleg Verniaiev     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angelina Melnikova </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caterina Barloggio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carina Kroell      </t>
-  </si>
-  <si>
     <t>Eythora Thorsdottir</t>
   </si>
   <si>
-    <t xml:space="preserve">Ilaria Käslin      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.B Lopez Arocha   </t>
-  </si>
-  <si>
-    <t>Parallel bars</t>
-  </si>
-  <si>
     <t>Vault</t>
   </si>
   <si>
-    <t>High bar</t>
-  </si>
-  <si>
     <t>Rings</t>
   </si>
   <si>
-    <t>Pommel horse</t>
-  </si>
-  <si>
     <t>Floor</t>
   </si>
   <si>
@@ -115,9 +74,6 @@
     <t>Bart Deurloo</t>
   </si>
   <si>
-    <t>James Hall</t>
-  </si>
-  <si>
     <t>Marcel Nguyen</t>
   </si>
   <si>
@@ -142,30 +98,15 @@
     <t>Julien Gobaux</t>
   </si>
   <si>
-    <t>Thea Brogli</t>
-  </si>
-  <si>
     <t>Angelina Melnikova</t>
   </si>
   <si>
     <t>Diana Varinska</t>
   </si>
   <si>
-    <t>Emily Thomas</t>
-  </si>
-  <si>
     <t>Ilaria Kaeslin</t>
   </si>
   <si>
-    <t>Isabela Onyshko</t>
-  </si>
-  <si>
-    <t>Kim Bui Germany</t>
-  </si>
-  <si>
-    <t>Leonie Meier</t>
-  </si>
-  <si>
     <t>Mélanie De Jesus Dos Santos</t>
   </si>
   <si>
@@ -188,12 +129,24 @@
   </si>
   <si>
     <t>Pommel Horse</t>
+  </si>
+  <si>
+    <t>Kim Bui</t>
+  </si>
+  <si>
+    <t>Caterina Barloggio</t>
+  </si>
+  <si>
+    <t>Anina Wildi</t>
+  </si>
+  <si>
+    <t>Jade Barbosa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -266,6 +219,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,11 +533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -596,7 +550,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,88 +558,113 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>31</v>
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>32</v>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>33</v>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C15">
-    <sortState ref="A5:C15">
+  <autoFilter ref="A4:C15" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A5:C14">
       <sortCondition ref="A4:A15"/>
     </sortState>
   </autoFilter>
@@ -694,7 +673,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Apparatus!$A$4:$A$9</xm:f>
           </x14:formula1>
@@ -707,11 +686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -724,7 +703,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,41 +711,53 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
+      <c r="B6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -774,60 +765,78 @@
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
-        <v>42</v>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
+      <c r="B12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
-        <v>45</v>
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>46</v>
+      <c r="B15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C13">
-    <sortState ref="A5:C13">
+  <autoFilter ref="A4:C13" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState ref="A5:C15">
       <sortCondition ref="A4:A13"/>
     </sortState>
   </autoFilter>
@@ -836,7 +845,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Apparatus!$A$12:$A$15</xm:f>
           </x14:formula1>
@@ -849,23 +858,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -880,76 +889,94 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
+        <f>M!$A$5</f>
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
+      <c r="B5" s="1" t="str">
+        <f>M!$B$5</f>
+        <v>Bart Deurloo</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>M!$C$5</f>
+        <v>Rings</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <f>M!$A$6</f>
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
+      <c r="B6" s="1" t="str">
+        <f>M!$B$6</f>
+        <v>Nikita Nagornyy</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>M!$C$6</f>
+        <v>Vault</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <f>M!$A$7</f>
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
+      <c r="B7" s="1" t="str">
+        <f>M!$B$7</f>
+        <v>Marcel Nguyen</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>M!$C$7</f>
+        <v>Vault</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
+        <f>M!$A$8</f>
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>M!$B$8</f>
+        <v>Pablo Brägger</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>M!$C$8</f>
+        <v>Horizontal Bar</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
+        <f>M!$A$9</f>
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
+      <c r="B9" s="1" t="str">
+        <f>M!$B$9</f>
+        <v>Oleg Verniaiev</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>M!$C$9</f>
+        <v>Parallel Bars</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
+        <f>M!$A$10</f>
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
+      <c r="B10" s="1" t="str">
+        <f>M!$B$10</f>
+        <v>Marian Dragulescu</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>M!$C$10</f>
+        <v>Pommel Horse</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -979,7 +1006,7 @@
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -994,76 +1021,94 @@
         <v>0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
+        <f>F!$A$5</f>
         <v>1</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
+      <c r="B23" s="4" t="str">
+        <f>F!$B$5</f>
+        <v>Caterina Barloggio</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>F!$C$5</f>
+        <v>Floor</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
+        <f>F!$A$6</f>
         <v>2</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
+      <c r="B24" s="4" t="str">
+        <f>F!$B$6</f>
+        <v>Anina Wildi</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>F!$C$6</f>
+        <v>Uneven bars</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
+        <f>F!$A$7</f>
         <v>3</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>23</v>
+      <c r="B25" s="4" t="str">
+        <f>F!$B$7</f>
+        <v>Jade Barbosa</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>F!$C$7</f>
+        <v>Floor</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>24</v>
+        <f>F!$A$8</f>
+        <v>4</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f>F!$B$8</f>
+        <v>Oksana Chusovitina</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f>F!$C$8</f>
+        <v>Balance Beam</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
+        <f>F!$A$9</f>
         <v>5</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>24</v>
+      <c r="B27" s="4" t="str">
+        <f>F!$B$9</f>
+        <v>Ilaria Kaeslin</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>F!$C$9</f>
+        <v>Floor</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
+        <f>F!$A$10</f>
         <v>6</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>23</v>
+      <c r="B28" s="4" t="str">
+        <f>F!$B$10</f>
+        <v>Diana Varinska</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f>F!$C$10</f>
+        <v>Floor</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1088,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1097,62 +1142,62 @@
   <sheetData>
     <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XLS per attrezzo finale (MG 2018)
</commit_message>
<xml_diff>
--- a/docs/OrdinePartenzaFinale.xlsx
+++ b/docs/OrdinePartenzaFinale.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0amalor\Work folders\Roaming\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\MemorialGander\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6934A617-D059-4EBB-9233-AF2F18726A3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">M!$A$4:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'M+F'!$A$4:$C$15</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,11 +532,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -569,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,10 +579,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,10 +590,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,10 +612,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,34 +623,34 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +662,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C15" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A4:C15">
     <sortState ref="A5:C14">
       <sortCondition ref="A4:A15"/>
     </sortState>
@@ -673,7 +672,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Apparatus!$A$4:$A$9</xm:f>
           </x14:formula1>
@@ -686,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -722,10 +721,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,10 +732,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,10 +743,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -777,7 +776,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -786,34 +785,34 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="8" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -822,10 +821,10 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +834,7 @@
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C13" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A4:C13">
     <sortState ref="A5:C15">
       <sortCondition ref="A4:A13"/>
     </sortState>
@@ -845,7 +844,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Apparatus!$A$12:$A$15</xm:f>
           </x14:formula1>
@@ -858,11 +857,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -902,11 +901,11 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>M!$B$5</f>
-        <v>Bart Deurloo</v>
+        <v>Marian Dragulescu</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>M!$C$5</f>
-        <v>Rings</v>
+        <v>Pommel Horse</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -916,11 +915,11 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>M!$B$6</f>
-        <v>Nikita Nagornyy</v>
+        <v>Pablo Brägger</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>M!$C$6</f>
-        <v>Vault</v>
+        <v>Horizontal Bar</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -930,11 +929,11 @@
       </c>
       <c r="B7" s="1" t="str">
         <f>M!$B$7</f>
-        <v>Marcel Nguyen</v>
+        <v>Julien Gobaux</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>M!$C$7</f>
-        <v>Vault</v>
+        <v>Rings</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -944,11 +943,11 @@
       </c>
       <c r="B8" s="1" t="str">
         <f>M!$B$8</f>
-        <v>Pablo Brägger</v>
+        <v>Oliver Hegi</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>M!$C$8</f>
-        <v>Horizontal Bar</v>
+        <v>Vault</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -958,11 +957,11 @@
       </c>
       <c r="B9" s="1" t="str">
         <f>M!$B$9</f>
-        <v>Oleg Verniaiev</v>
+        <v>Nikita Nagornyy</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>M!$C$9</f>
-        <v>Parallel Bars</v>
+        <v>Vault</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -972,11 +971,11 @@
       </c>
       <c r="B10" s="1" t="str">
         <f>M!$B$10</f>
-        <v>Marian Dragulescu</v>
+        <v>Marcel Nguyen</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>M!$C$10</f>
-        <v>Pommel Horse</v>
+        <v>Vault</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1032,13 +1031,13 @@
         <f>F!$A$5</f>
         <v>1</v>
       </c>
-      <c r="B23" s="4" t="str">
+      <c r="B23" s="6" t="str">
         <f>F!$B$5</f>
-        <v>Caterina Barloggio</v>
-      </c>
-      <c r="C23" s="4" t="str">
+        <v>Angelina Melnikova</v>
+      </c>
+      <c r="C23" s="6" t="str">
         <f>F!$C$5</f>
-        <v>Floor</v>
+        <v>Vault</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1046,13 +1045,13 @@
         <f>F!$A$6</f>
         <v>2</v>
       </c>
-      <c r="B24" s="4" t="str">
+      <c r="B24" s="6" t="str">
         <f>F!$B$6</f>
-        <v>Anina Wildi</v>
-      </c>
-      <c r="C24" s="4" t="str">
+        <v>Kim Bui</v>
+      </c>
+      <c r="C24" s="6" t="str">
         <f>F!$C$6</f>
-        <v>Uneven bars</v>
+        <v>Floor</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1060,13 +1059,13 @@
         <f>F!$A$7</f>
         <v>3</v>
       </c>
-      <c r="B25" s="4" t="str">
+      <c r="B25" s="6" t="str">
         <f>F!$B$7</f>
-        <v>Jade Barbosa</v>
-      </c>
-      <c r="C25" s="4" t="str">
+        <v xml:space="preserve">Flávia Lopes Saraiva </v>
+      </c>
+      <c r="C25" s="6" t="str">
         <f>F!$C$7</f>
-        <v>Floor</v>
+        <v>Vault</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1074,13 +1073,13 @@
         <f>F!$A$8</f>
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="str">
+      <c r="B26" s="6" t="str">
         <f>F!$B$8</f>
-        <v>Oksana Chusovitina</v>
-      </c>
-      <c r="C26" s="4" t="str">
+        <v>Eythora Thorsdottir</v>
+      </c>
+      <c r="C26" s="6" t="str">
         <f>F!$C$8</f>
-        <v>Balance Beam</v>
+        <v>Floor</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -1088,11 +1087,11 @@
         <f>F!$A$9</f>
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="str">
+      <c r="B27" s="6" t="str">
         <f>F!$B$9</f>
-        <v>Ilaria Kaeslin</v>
-      </c>
-      <c r="C27" s="4" t="str">
+        <v>Diana Varinska</v>
+      </c>
+      <c r="C27" s="6" t="str">
         <f>F!$C$9</f>
         <v>Floor</v>
       </c>
@@ -1102,11 +1101,11 @@
         <f>F!$A$10</f>
         <v>6</v>
       </c>
-      <c r="B28" s="4" t="str">
+      <c r="B28" s="6" t="str">
         <f>F!$B$10</f>
-        <v>Diana Varinska</v>
-      </c>
-      <c r="C28" s="4" t="str">
+        <v>Jade Barbosa</v>
+      </c>
+      <c r="C28" s="6" t="str">
         <f>F!$C$10</f>
         <v>Floor</v>
       </c>
@@ -1133,7 +1132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>